<commit_message>
reorganisation of folder structure
</commit_message>
<xml_diff>
--- a/5_taxonomy/COI_barcodes_only_taxonomies_20180410.xlsx
+++ b/5_taxonomy/COI_barcodes_only_taxonomies_20180410.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10701"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Roslin_Greenland/2017/bulk_samples/mapping_git/5_taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD09C7B6-4455-934A-872F-387456E83844}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9DEC7A-8C8E-6046-B87D-4C18D656DC16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="29360" windowHeight="23560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4900" yWindow="440" windowWidth="29360" windowHeight="23560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COI_Barcodes" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COI_Barcodes!$A$1:$F$397</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="916">
   <si>
     <t>Barcode_code</t>
   </si>
@@ -2781,6 +2781,9 @@
   </si>
   <si>
     <t>Spilogona arcticola</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -2915,7 +2918,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2967,7 +2970,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3172,8 +3175,8 @@
   <dimension ref="A1:F397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F397"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3217,7 +3220,9 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E2" s="2" t="str">
         <f>IFERROR(RIGHT(D2, LEN(D2)-IFERROR(FIND(" ", D2),"")), "NA")</f>
         <v>NA</v>
@@ -3256,15 +3261,19 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15">
@@ -3299,7 +3308,9 @@
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3319,7 +3330,9 @@
       <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3361,7 +3374,9 @@
       <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3378,15 +3393,19 @@
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15">
@@ -3421,7 +3440,9 @@
       <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3441,7 +3462,9 @@
       <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3461,7 +3484,9 @@
       <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3478,15 +3503,19 @@
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15">
@@ -3540,15 +3569,19 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -3561,7 +3594,9 @@
       <c r="C19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3578,15 +3613,19 @@
       <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Trichoceridae_NA</v>
+        <v>Trichoceridae_NA_NA</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15">
@@ -3599,7 +3638,9 @@
       <c r="C21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3641,7 +3682,9 @@
       <c r="C23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3661,7 +3704,9 @@
       <c r="C24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3681,7 +3726,9 @@
       <c r="C25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3723,7 +3770,9 @@
       <c r="C27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3743,7 +3792,9 @@
       <c r="C28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3763,7 +3814,9 @@
       <c r="C29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3802,15 +3855,19 @@
       <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Ichneumonidae_NA</v>
+        <v>Ichneumonidae_NA_NA</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15">
@@ -3823,7 +3880,9 @@
       <c r="C32" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3843,7 +3902,9 @@
       <c r="C33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3863,7 +3924,9 @@
       <c r="C34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3905,7 +3968,9 @@
       <c r="C36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3925,7 +3990,9 @@
       <c r="C37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -3945,7 +4012,9 @@
       <c r="C38" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4097,7 +4166,9 @@
       <c r="C45" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4139,7 +4210,9 @@
       <c r="C47" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4159,7 +4232,9 @@
       <c r="C48" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4198,15 +4273,19 @@
       <c r="B50" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
       <c r="F50" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Penthaleidae_NA</v>
+        <v>Penthaleidae_NA_NA</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15">
@@ -4285,7 +4364,9 @@
       <c r="C54" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="3"/>
+      <c r="D54" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E54" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4327,7 +4408,9 @@
       <c r="C56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E56" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4347,7 +4430,9 @@
       <c r="C57" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E57" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4367,7 +4452,9 @@
       <c r="C58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E58" s="2" t="str">
         <f t="shared" si="0"/>
         <v>NA</v>
@@ -4431,7 +4518,9 @@
       <c r="C61" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E61" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4451,7 +4540,9 @@
       <c r="C62" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E62" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4493,7 +4584,9 @@
       <c r="C64" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D64" s="3"/>
+      <c r="D64" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E64" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4535,7 +4628,9 @@
       <c r="C66" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D66" s="3"/>
+      <c r="D66" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E66" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4574,15 +4669,19 @@
       <c r="B68" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E68" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="F68" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15">
@@ -4595,7 +4694,9 @@
       <c r="C69" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E69" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4637,7 +4738,9 @@
       <c r="C71" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="3"/>
+      <c r="D71" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E71" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4698,15 +4801,19 @@
       <c r="B74" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E74" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="F74" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Canacidae_NA</v>
+        <v>Canacidae_NA_NA</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15">
@@ -4785,7 +4892,9 @@
       <c r="C78" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E78" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4824,15 +4933,19 @@
       <c r="B80" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E80" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="F80" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Ichneumonidae_NA</v>
+        <v>Ichneumonidae_NA_NA</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15">
@@ -4845,7 +4958,9 @@
       <c r="C81" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D81" s="3"/>
+      <c r="D81" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E81" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4931,7 +5046,9 @@
       <c r="C85" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E85" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4951,7 +5068,9 @@
       <c r="C86" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D86" s="3"/>
+      <c r="D86" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E86" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4971,7 +5090,9 @@
       <c r="C87" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E87" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -4991,7 +5112,9 @@
       <c r="C88" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D88" s="3"/>
+      <c r="D88" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E88" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5033,7 +5156,9 @@
       <c r="C90" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E90" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5053,7 +5178,9 @@
       <c r="C91" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E91" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5073,7 +5200,9 @@
       <c r="C92" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E92" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5137,7 +5266,9 @@
       <c r="C95" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E95" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5311,7 +5442,9 @@
       <c r="C103" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D103" s="3"/>
+      <c r="D103" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E103" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5394,15 +5527,19 @@
       <c r="B107" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="C107" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E107" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="F107" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Mycetophilidae_NA</v>
+        <v>Mycetophilidae_NA_NA</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15">
@@ -5437,7 +5574,9 @@
       <c r="C109" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D109" s="3"/>
+      <c r="D109" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E109" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5457,7 +5596,9 @@
       <c r="C110" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D110" s="3"/>
+      <c r="D110" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E110" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5521,7 +5662,9 @@
       <c r="C113" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E113" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5585,7 +5728,9 @@
       <c r="C116" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E116" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
@@ -5624,15 +5769,19 @@
       <c r="B118" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="C118" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E118" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="F118" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Sciaridae_NA</v>
+        <v>Sciaridae_NA_NA</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="15">
@@ -5642,15 +5791,19 @@
       <c r="B119" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="C119" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E119" s="2" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="F119" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15">
@@ -5726,15 +5879,19 @@
       <c r="B123" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="C123" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E123" s="2" t="str">
         <f t="shared" ref="E123:E184" si="4">IFERROR(RIGHT(D123, LEN(D123)-IFERROR(FIND(" ", D123),"")), "NA")</f>
         <v>NA</v>
       </c>
       <c r="F123" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15">
@@ -5744,15 +5901,19 @@
       <c r="B124" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="C124" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E124" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
       <c r="F124" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Agromyzidae_NA</v>
+        <v>Agromyzidae_NA_NA</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15">
@@ -5765,7 +5926,9 @@
       <c r="C125" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D125" s="3"/>
+      <c r="D125" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E125" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -5873,7 +6036,9 @@
       <c r="C130" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D130" s="3"/>
+      <c r="D130" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E130" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -5937,7 +6102,9 @@
       <c r="C133" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D133" s="3"/>
+      <c r="D133" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E133" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -5957,7 +6124,9 @@
       <c r="C134" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D134" s="3"/>
+      <c r="D134" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E134" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6021,7 +6190,9 @@
       <c r="C137" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D137" s="3"/>
+      <c r="D137" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E137" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6041,7 +6212,9 @@
       <c r="C138" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D138" s="3"/>
+      <c r="D138" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E138" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6061,7 +6234,9 @@
       <c r="C139" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D139" s="3"/>
+      <c r="D139" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E139" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6081,7 +6256,9 @@
       <c r="C140" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D140" s="3"/>
+      <c r="D140" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E140" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6255,7 +6432,9 @@
       <c r="C148" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D148" s="3"/>
+      <c r="D148" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E148" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6319,7 +6498,9 @@
       <c r="C151" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D151" s="3"/>
+      <c r="D151" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E151" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6336,15 +6517,19 @@
       <c r="B152" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
+      <c r="C152" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E152" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
       <c r="F152" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="15">
@@ -6401,7 +6586,9 @@
       <c r="C155" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D155" s="3"/>
+      <c r="D155" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E155" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6440,15 +6627,19 @@
       <c r="B157" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
+      <c r="C157" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E157" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
       <c r="F157" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>Eupodidae_NA</v>
+        <v>Eupodidae_NA_NA</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="15">
@@ -6461,7 +6652,9 @@
       <c r="C158" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D158" s="3"/>
+      <c r="D158" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E158" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6478,15 +6671,19 @@
       <c r="B159" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
+      <c r="C159" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E159" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
       <c r="F159" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>Eupodidae_NA</v>
+        <v>Eupodidae_NA_NA</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="15">
@@ -6631,7 +6828,9 @@
       <c r="C166" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="D166" s="3"/>
+      <c r="D166" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E166" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6695,7 +6894,9 @@
       <c r="C169" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D169" s="3"/>
+      <c r="D169" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E169" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6715,7 +6916,9 @@
       <c r="C170" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D170" s="3"/>
+      <c r="D170" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E170" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6735,7 +6938,9 @@
       <c r="C171" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D171" s="3"/>
+      <c r="D171" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E171" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6953,7 +7158,9 @@
       <c r="C181" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D181" s="3"/>
+      <c r="D181" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E181" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6973,7 +7180,9 @@
       <c r="C182" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="D182" s="3"/>
+      <c r="D182" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E182" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -6993,7 +7202,9 @@
       <c r="C183" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="D183" s="3"/>
+      <c r="D183" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E183" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
@@ -7123,7 +7334,9 @@
       <c r="C189" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D189" s="3"/>
+      <c r="D189" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E189" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7165,7 +7378,9 @@
       <c r="C191" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="D191" s="3"/>
+      <c r="D191" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E191" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7229,7 +7444,9 @@
       <c r="C194" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="D194" s="3"/>
+      <c r="D194" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E194" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7249,7 +7466,9 @@
       <c r="C195" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="D195" s="3"/>
+      <c r="D195" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E195" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7269,7 +7488,9 @@
       <c r="C196" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D196" s="3"/>
+      <c r="D196" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E196" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7289,7 +7510,9 @@
       <c r="C197" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D197" s="3"/>
+      <c r="D197" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E197" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7331,7 +7554,9 @@
       <c r="C199" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D199" s="3"/>
+      <c r="D199" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E199" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7483,7 +7708,9 @@
       <c r="C206" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="D206" s="3"/>
+      <c r="D206" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E206" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7503,7 +7730,9 @@
       <c r="C207" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D207" s="3"/>
+      <c r="D207" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E207" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7523,7 +7752,9 @@
       <c r="C208" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="D208" s="3"/>
+      <c r="D208" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E208" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7628,15 +7859,19 @@
       <c r="B213" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C213" s="3"/>
-      <c r="D213" s="3"/>
+      <c r="C213" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E213" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
       </c>
       <c r="F213" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>Lebertiidae_NA</v>
+        <v>Lebertiidae_NA_NA</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="15">
@@ -7646,15 +7881,19 @@
       <c r="B214" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3"/>
+      <c r="C214" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E214" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
       </c>
       <c r="F214" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>Erythraeidae_NA</v>
+        <v>Erythraeidae_NA_NA</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="15">
@@ -7708,15 +7947,19 @@
       <c r="B217" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
+      <c r="C217" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E217" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
       </c>
       <c r="F217" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>Chironomidae_NA</v>
+        <v>Chironomidae_NA_NA</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="15">
@@ -7751,7 +7994,9 @@
       <c r="C219" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D219" s="3"/>
+      <c r="D219" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E219" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7881,7 +8126,9 @@
       <c r="C225" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D225" s="3"/>
+      <c r="D225" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E225" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7945,7 +8192,9 @@
       <c r="C228" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D228" s="3"/>
+      <c r="D228" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E228" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -7987,7 +8236,9 @@
       <c r="C230" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D230" s="3"/>
+      <c r="D230" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E230" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8029,7 +8280,9 @@
       <c r="C232" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D232" s="3"/>
+      <c r="D232" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E232" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8203,7 +8456,9 @@
       <c r="C240" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D240" s="3"/>
+      <c r="D240" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E240" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8311,7 +8566,9 @@
       <c r="C245" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="D245" s="3"/>
+      <c r="D245" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E245" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8331,7 +8588,9 @@
       <c r="C246" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D246" s="3"/>
+      <c r="D246" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E246" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8351,7 +8610,9 @@
       <c r="C247" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="D247" s="3"/>
+      <c r="D247" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E247" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8371,7 +8632,9 @@
       <c r="C248" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D248" s="3"/>
+      <c r="D248" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E248" s="2" t="str">
         <f t="shared" ref="E248:E310" si="8">IFERROR(RIGHT(D248, LEN(D248)-IFERROR(FIND(" ", D248),"")), "NA")</f>
         <v>NA</v>
@@ -8501,7 +8764,9 @@
       <c r="C254" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D254" s="3"/>
+      <c r="D254" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E254" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -8829,7 +9094,9 @@
       <c r="C269" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D269" s="3"/>
+      <c r="D269" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E269" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -8849,7 +9116,9 @@
       <c r="C270" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D270" s="3"/>
+      <c r="D270" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E270" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -9397,7 +9666,9 @@
       <c r="C295" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D295" s="3"/>
+      <c r="D295" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E295" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -9505,7 +9776,9 @@
       <c r="C300" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D300" s="3"/>
+      <c r="D300" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E300" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -9569,7 +9842,9 @@
       <c r="C303" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D303" s="3"/>
+      <c r="D303" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E303" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -9611,7 +9886,9 @@
       <c r="C305" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D305" s="3"/>
+      <c r="D305" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E305" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
@@ -10291,7 +10568,9 @@
       <c r="C336" s="3" t="s">
         <v>744</v>
       </c>
-      <c r="D336" s="3"/>
+      <c r="D336" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E336" s="2" t="str">
         <f t="shared" si="10"/>
         <v>NA</v>
@@ -10990,15 +11269,19 @@
       <c r="B368" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C368" s="3"/>
-      <c r="D368" s="3"/>
+      <c r="C368" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D368" s="3" t="s">
+        <v>915</v>
+      </c>
       <c r="E368" s="2" t="str">
         <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="F368" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>Ichneumonidae_NA</v>
+        <v>Ichneumonidae_NA_NA</v>
       </c>
     </row>
     <row r="369" spans="1:6" ht="15">

</xml_diff>